<commit_message>
Removed sharelatex link for future markdown pushes.
</commit_message>
<xml_diff>
--- a/Personal Time Tracking/Phil Oetinger.xlsx
+++ b/Personal Time Tracking/Phil Oetinger.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>DATE</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Familiarization with last week's missed work. Read through documentation from 2017.</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,7 +122,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
@@ -402,17 +411,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" thickTop="1" thickBottom="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="2"/>
-    <col min="3" max="3" width="92.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="232" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -426,6 +435,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
+        <v>43157</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>